<commit_message>
Added user created data
</commit_message>
<xml_diff>
--- a/notebooks/personas_pob_total_AGLO.xlsx
+++ b/notebooks/personas_pob_total_AGLO.xlsx
@@ -534,28 +534,28 @@
         <v>35</v>
       </c>
       <c r="C2">
-        <v>83.7</v>
+        <v>84.2</v>
       </c>
       <c r="D2">
-        <v>98.3</v>
+        <v>97.40000000000001</v>
       </c>
       <c r="E2">
-        <v>90.90000000000001</v>
+        <v>90.8</v>
       </c>
       <c r="F2">
-        <v>92.59999999999999</v>
+        <v>93.5</v>
       </c>
       <c r="G2">
-        <v>76.7</v>
+        <v>77.3</v>
       </c>
       <c r="H2">
-        <v>89.2</v>
+        <v>89.3</v>
       </c>
       <c r="I2">
-        <v>87.40000000000001</v>
+        <v>86.90000000000001</v>
       </c>
       <c r="J2">
-        <v>84.3</v>
+        <v>83.90000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -596,28 +596,28 @@
         <v>35</v>
       </c>
       <c r="C4">
-        <v>446.3</v>
+        <v>450.7</v>
       </c>
       <c r="D4">
-        <v>493.7</v>
+        <v>494.1</v>
       </c>
       <c r="E4">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F4">
-        <v>456.3</v>
+        <v>457.2</v>
       </c>
       <c r="G4">
-        <v>407.4</v>
+        <v>403</v>
       </c>
       <c r="H4">
-        <v>487.1</v>
+        <v>491.2</v>
       </c>
       <c r="I4">
-        <v>373.8</v>
+        <v>373.1</v>
       </c>
       <c r="J4">
-        <v>406.6</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -658,25 +658,25 @@
         <v>35</v>
       </c>
       <c r="C6">
-        <v>64.59999999999999</v>
+        <v>64.7</v>
       </c>
       <c r="D6">
-        <v>76.8</v>
+        <v>76.09999999999999</v>
       </c>
       <c r="E6">
-        <v>67.90000000000001</v>
+        <v>68.40000000000001</v>
       </c>
       <c r="F6">
-        <v>69.5</v>
+        <v>70</v>
       </c>
       <c r="G6">
         <v>60.2</v>
       </c>
       <c r="H6">
-        <v>77.09999999999999</v>
+        <v>77.5</v>
       </c>
       <c r="I6">
-        <v>66.09999999999999</v>
+        <v>65.7</v>
       </c>
       <c r="J6">
         <v>75.90000000000001</v>
@@ -720,25 +720,25 @@
         <v>35</v>
       </c>
       <c r="C8">
-        <v>29.8</v>
+        <v>29.6</v>
       </c>
       <c r="D8">
-        <v>35</v>
+        <v>35.6</v>
       </c>
       <c r="E8">
-        <v>30.2</v>
+        <v>31</v>
       </c>
       <c r="F8">
-        <v>37</v>
+        <v>36.6</v>
       </c>
       <c r="G8">
-        <v>35.9</v>
+        <v>35.8</v>
       </c>
       <c r="H8">
-        <v>45.7</v>
+        <v>45.9</v>
       </c>
       <c r="I8">
-        <v>34.7</v>
+        <v>35.5</v>
       </c>
       <c r="J8">
         <v>41.9</v>
@@ -782,25 +782,25 @@
         <v>35</v>
       </c>
       <c r="C10">
-        <v>70.5</v>
+        <v>70.2</v>
       </c>
       <c r="D10">
-        <v>80.09999999999999</v>
+        <v>82.09999999999999</v>
       </c>
       <c r="E10">
         <v>70.7</v>
       </c>
       <c r="F10">
-        <v>74.5</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="G10">
-        <v>65</v>
+        <v>64.90000000000001</v>
       </c>
       <c r="H10">
-        <v>80.59999999999999</v>
+        <v>79.90000000000001</v>
       </c>
       <c r="I10">
-        <v>71.5</v>
+        <v>71.59999999999999</v>
       </c>
       <c r="J10">
         <v>78.7</v>
@@ -844,28 +844,28 @@
         <v>35</v>
       </c>
       <c r="C12">
-        <v>472.4</v>
+        <v>470.5</v>
       </c>
       <c r="D12">
-        <v>523.9</v>
+        <v>525.2</v>
       </c>
       <c r="E12">
-        <v>484.1</v>
+        <v>480.5</v>
       </c>
       <c r="F12">
-        <v>489.2</v>
+        <v>489.3</v>
       </c>
       <c r="G12">
-        <v>443.6</v>
+        <v>443</v>
       </c>
       <c r="H12">
-        <v>545.8</v>
+        <v>542.4</v>
       </c>
       <c r="I12">
-        <v>446.4</v>
+        <v>446.2</v>
       </c>
       <c r="J12">
-        <v>459.4</v>
+        <v>459.6</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -906,28 +906,28 @@
         <v>35</v>
       </c>
       <c r="C14">
-        <v>158.4</v>
+        <v>157.4</v>
       </c>
       <c r="D14">
-        <v>170.4</v>
+        <v>169.5</v>
       </c>
       <c r="E14">
-        <v>154</v>
+        <v>153.8</v>
       </c>
       <c r="F14">
-        <v>171.1</v>
+        <v>170.2</v>
       </c>
       <c r="G14">
-        <v>162.1</v>
+        <v>161.2</v>
       </c>
       <c r="H14">
-        <v>162.4</v>
+        <v>162.8</v>
       </c>
       <c r="I14">
-        <v>160.6</v>
+        <v>160.4</v>
       </c>
       <c r="J14">
-        <v>160.3</v>
+        <v>160.8</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -968,22 +968,22 @@
         <v>35</v>
       </c>
       <c r="C16">
-        <v>102.4</v>
+        <v>101.2</v>
       </c>
       <c r="D16">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E16">
-        <v>102.8</v>
+        <v>103.5</v>
       </c>
       <c r="F16">
-        <v>107.9</v>
+        <v>107.7</v>
       </c>
       <c r="G16">
         <v>111.4</v>
       </c>
       <c r="H16">
-        <v>121</v>
+        <v>120.5</v>
       </c>
       <c r="I16">
         <v>115.1</v>
@@ -1030,28 +1030,28 @@
         <v>35</v>
       </c>
       <c r="C18">
-        <v>7169.2</v>
+        <v>7165.4</v>
       </c>
       <c r="D18">
-        <v>7832.7</v>
+        <v>7832.2</v>
       </c>
       <c r="E18">
-        <v>7214.3</v>
+        <v>7209.6</v>
       </c>
       <c r="F18">
-        <v>7673.5</v>
+        <v>7681.7</v>
       </c>
       <c r="G18">
-        <v>6928.1</v>
+        <v>6930.8</v>
       </c>
       <c r="H18">
-        <v>7735.7</v>
+        <v>7730.5</v>
       </c>
       <c r="I18">
-        <v>7069.3</v>
+        <v>7072.2</v>
       </c>
       <c r="J18">
-        <v>7326.2</v>
+        <v>7326</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1092,28 +1092,28 @@
         <v>35</v>
       </c>
       <c r="C20">
-        <v>4113.5</v>
+        <v>4119.8</v>
       </c>
       <c r="D20">
-        <v>4426.3</v>
+        <v>4425.5</v>
       </c>
       <c r="E20">
-        <v>3960.3</v>
+        <v>3961.6</v>
       </c>
       <c r="F20">
-        <v>4281.9</v>
+        <v>4285.6</v>
       </c>
       <c r="G20">
-        <v>3907.1</v>
+        <v>3911.2</v>
       </c>
       <c r="H20">
-        <v>4270.4</v>
+        <v>4273</v>
       </c>
       <c r="I20">
-        <v>3844.9</v>
+        <v>3836.6</v>
       </c>
       <c r="J20">
-        <v>3997.7</v>
+        <v>3996.6</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1154,28 +1154,28 @@
         <v>35</v>
       </c>
       <c r="C22">
-        <v>119.2</v>
+        <v>124.3</v>
       </c>
       <c r="D22">
-        <v>147.4</v>
+        <v>147.6</v>
       </c>
       <c r="E22">
-        <v>131.7</v>
+        <v>131.9</v>
       </c>
       <c r="F22">
-        <v>137</v>
+        <v>136.4</v>
       </c>
       <c r="G22">
-        <v>111.3</v>
+        <v>111.5</v>
       </c>
       <c r="H22">
-        <v>130</v>
+        <v>131.4</v>
       </c>
       <c r="I22">
-        <v>115.3</v>
+        <v>114.4</v>
       </c>
       <c r="J22">
-        <v>129.9</v>
+        <v>130.2</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1216,28 +1216,28 @@
         <v>35</v>
       </c>
       <c r="C24">
-        <v>240.4</v>
+        <v>236.2</v>
       </c>
       <c r="D24">
-        <v>266.3</v>
+        <v>267.4</v>
       </c>
       <c r="E24">
-        <v>233.5</v>
+        <v>233.7</v>
       </c>
       <c r="F24">
-        <v>262.1</v>
+        <v>261.9</v>
       </c>
       <c r="G24">
-        <v>191</v>
+        <v>193.1</v>
       </c>
       <c r="H24">
-        <v>246.8</v>
+        <v>247.4</v>
       </c>
       <c r="I24">
-        <v>208.2</v>
+        <v>209.1</v>
       </c>
       <c r="J24">
-        <v>216.1</v>
+        <v>216.5</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1278,25 +1278,25 @@
         <v>35</v>
       </c>
       <c r="C26">
-        <v>82.3</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="D26">
-        <v>87.90000000000001</v>
+        <v>88.8</v>
       </c>
       <c r="E26">
-        <v>77.09999999999999</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="F26">
-        <v>91</v>
+        <v>91.3</v>
       </c>
       <c r="G26">
-        <v>74.40000000000001</v>
+        <v>73.59999999999999</v>
       </c>
       <c r="H26">
-        <v>86.5</v>
+        <v>85.7</v>
       </c>
       <c r="I26">
-        <v>77.09999999999999</v>
+        <v>77.3</v>
       </c>
       <c r="J26">
         <v>89.3</v>
@@ -1340,28 +1340,28 @@
         <v>35</v>
       </c>
       <c r="C28">
-        <v>194.6</v>
+        <v>195.1</v>
       </c>
       <c r="D28">
         <v>212.6</v>
       </c>
       <c r="E28">
-        <v>189.1</v>
+        <v>192.2</v>
       </c>
       <c r="F28">
-        <v>199.3</v>
+        <v>200.1</v>
       </c>
       <c r="G28">
-        <v>162.3</v>
+        <v>162</v>
       </c>
       <c r="H28">
-        <v>180.1</v>
+        <v>182.2</v>
       </c>
       <c r="I28">
-        <v>149.6</v>
+        <v>149.8</v>
       </c>
       <c r="J28">
-        <v>174.5</v>
+        <v>174.7</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1402,28 +1402,28 @@
         <v>35</v>
       </c>
       <c r="C30">
-        <v>339.2</v>
+        <v>341.6</v>
       </c>
       <c r="D30">
         <v>388</v>
       </c>
       <c r="E30">
-        <v>339.5</v>
+        <v>341.1</v>
       </c>
       <c r="F30">
-        <v>399.3</v>
+        <v>397.7</v>
       </c>
       <c r="G30">
-        <v>318.6</v>
+        <v>317</v>
       </c>
       <c r="H30">
         <v>356</v>
       </c>
       <c r="I30">
-        <v>323.9</v>
+        <v>324</v>
       </c>
       <c r="J30">
-        <v>341.8</v>
+        <v>342.1</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1464,25 +1464,25 @@
         <v>35</v>
       </c>
       <c r="C32">
-        <v>117.3</v>
+        <v>115.2</v>
       </c>
       <c r="D32">
-        <v>111.8</v>
+        <v>112.1</v>
       </c>
       <c r="E32">
-        <v>111.9</v>
+        <v>110.4</v>
       </c>
       <c r="F32">
-        <v>119.1</v>
+        <v>118.8</v>
       </c>
       <c r="G32">
-        <v>113</v>
+        <v>111.5</v>
       </c>
       <c r="H32">
-        <v>123.3</v>
+        <v>123.6</v>
       </c>
       <c r="I32">
-        <v>99.09999999999999</v>
+        <v>98.8</v>
       </c>
       <c r="J32">
         <v>98.59999999999999</v>
@@ -1526,28 +1526,28 @@
         <v>35</v>
       </c>
       <c r="C34">
-        <v>91.8</v>
+        <v>91.2</v>
       </c>
       <c r="D34">
-        <v>102.3</v>
+        <v>101.5</v>
       </c>
       <c r="E34">
-        <v>96.5</v>
+        <v>97.40000000000001</v>
       </c>
       <c r="F34">
-        <v>109.1</v>
+        <v>108.7</v>
       </c>
       <c r="G34">
-        <v>92.8</v>
+        <v>93.09999999999999</v>
       </c>
       <c r="H34">
-        <v>110.3</v>
+        <v>110.2</v>
       </c>
       <c r="I34">
         <v>95.59999999999999</v>
       </c>
       <c r="J34">
-        <v>100.3</v>
+        <v>100.9</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1588,25 +1588,25 @@
         <v>35</v>
       </c>
       <c r="C36">
-        <v>142.3</v>
+        <v>140.5</v>
       </c>
       <c r="D36">
-        <v>153.8</v>
+        <v>153.9</v>
       </c>
       <c r="E36">
-        <v>129.3</v>
+        <v>129.5</v>
       </c>
       <c r="F36">
-        <v>144.4</v>
+        <v>144.5</v>
       </c>
       <c r="G36">
-        <v>117</v>
+        <v>117.6</v>
       </c>
       <c r="H36">
-        <v>132.5</v>
+        <v>133.4</v>
       </c>
       <c r="I36">
-        <v>127.4</v>
+        <v>126.6</v>
       </c>
       <c r="J36">
         <v>128.7</v>
@@ -1650,25 +1650,25 @@
         <v>35</v>
       </c>
       <c r="C38">
-        <v>31.5</v>
+        <v>30.3</v>
       </c>
       <c r="D38">
-        <v>38.1</v>
+        <v>38.3</v>
       </c>
       <c r="E38">
-        <v>28.6</v>
+        <v>29.6</v>
       </c>
       <c r="F38">
-        <v>33.6</v>
+        <v>34.8</v>
       </c>
       <c r="G38">
-        <v>37.2</v>
+        <v>37.4</v>
       </c>
       <c r="H38">
         <v>39.6</v>
       </c>
       <c r="I38">
-        <v>36.2</v>
+        <v>36.6</v>
       </c>
       <c r="J38">
         <v>41.5</v>
@@ -1712,28 +1712,28 @@
         <v>35</v>
       </c>
       <c r="C40">
-        <v>169.6</v>
+        <v>170.3</v>
       </c>
       <c r="D40">
-        <v>209.1</v>
+        <v>208.7</v>
       </c>
       <c r="E40">
-        <v>187.5</v>
+        <v>187.4</v>
       </c>
       <c r="F40">
-        <v>200.3</v>
+        <v>199.2</v>
       </c>
       <c r="G40">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H40">
-        <v>211.2</v>
+        <v>210.5</v>
       </c>
       <c r="I40">
-        <v>193.1</v>
+        <v>193.4</v>
       </c>
       <c r="J40">
-        <v>195.6</v>
+        <v>195.1</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1774,13 +1774,13 @@
         <v>35</v>
       </c>
       <c r="C42">
-        <v>48.3</v>
+        <v>48.5</v>
       </c>
       <c r="D42">
-        <v>49</v>
+        <v>49.7</v>
       </c>
       <c r="E42">
-        <v>48.9</v>
+        <v>49.8</v>
       </c>
       <c r="F42">
         <v>50.1</v>
@@ -1789,10 +1789,10 @@
         <v>50.1</v>
       </c>
       <c r="H42">
-        <v>57.6</v>
+        <v>58</v>
       </c>
       <c r="I42">
-        <v>50.4</v>
+        <v>50.9</v>
       </c>
       <c r="J42">
         <v>51.7</v>
@@ -1836,28 +1836,28 @@
         <v>35</v>
       </c>
       <c r="C44">
-        <v>24.7</v>
+        <v>25.1</v>
       </c>
       <c r="D44">
-        <v>25.3</v>
+        <v>25.5</v>
       </c>
       <c r="E44">
-        <v>23.2</v>
+        <v>23.3</v>
       </c>
       <c r="F44">
-        <v>29</v>
+        <v>28.9</v>
       </c>
       <c r="G44">
         <v>19.4</v>
       </c>
       <c r="H44">
-        <v>22.8</v>
+        <v>22.6</v>
       </c>
       <c r="I44">
-        <v>18.6</v>
+        <v>18.9</v>
       </c>
       <c r="J44">
-        <v>20.9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1898,25 +1898,25 @@
         <v>35</v>
       </c>
       <c r="C46">
-        <v>398.6</v>
+        <v>399.9</v>
       </c>
       <c r="D46">
-        <v>446.7</v>
+        <v>447.7</v>
       </c>
       <c r="E46">
-        <v>416.4</v>
+        <v>415.5</v>
       </c>
       <c r="F46">
-        <v>417.6</v>
+        <v>415.8</v>
       </c>
       <c r="G46">
-        <v>394.6</v>
+        <v>395.6</v>
       </c>
       <c r="H46">
-        <v>442.9</v>
+        <v>443.5</v>
       </c>
       <c r="I46">
-        <v>380.1</v>
+        <v>377.5</v>
       </c>
       <c r="J46">
         <v>423.7</v>
@@ -1963,22 +1963,22 @@
         <v>233.4</v>
       </c>
       <c r="D48">
-        <v>269.5</v>
+        <v>270</v>
       </c>
       <c r="E48">
-        <v>239.5</v>
+        <v>239</v>
       </c>
       <c r="F48">
-        <v>235.6</v>
+        <v>236.5</v>
       </c>
       <c r="G48">
-        <v>224.6</v>
+        <v>224.4</v>
       </c>
       <c r="H48">
-        <v>242.3</v>
+        <v>241.7</v>
       </c>
       <c r="I48">
-        <v>234</v>
+        <v>234.6</v>
       </c>
       <c r="J48">
         <v>253.2</v>
@@ -2022,25 +2022,25 @@
         <v>35</v>
       </c>
       <c r="C50">
-        <v>188</v>
+        <v>184.7</v>
       </c>
       <c r="D50">
-        <v>203.1</v>
+        <v>202.9</v>
       </c>
       <c r="E50">
-        <v>191.5</v>
+        <v>191.6</v>
       </c>
       <c r="F50">
-        <v>200</v>
+        <v>199.8</v>
       </c>
       <c r="G50">
-        <v>189.6</v>
+        <v>190</v>
       </c>
       <c r="H50">
-        <v>213.9</v>
+        <v>214.5</v>
       </c>
       <c r="I50">
-        <v>158.8</v>
+        <v>158</v>
       </c>
       <c r="J50">
         <v>196.6</v>
@@ -2084,28 +2084,28 @@
         <v>35</v>
       </c>
       <c r="C52">
-        <v>78.90000000000001</v>
+        <v>79.90000000000001</v>
       </c>
       <c r="D52">
-        <v>93.7</v>
+        <v>93.09999999999999</v>
       </c>
       <c r="E52">
         <v>80.3</v>
       </c>
       <c r="F52">
-        <v>98.2</v>
+        <v>97.7</v>
       </c>
       <c r="G52">
-        <v>79.59999999999999</v>
+        <v>79.7</v>
       </c>
       <c r="H52">
-        <v>86.09999999999999</v>
+        <v>86.5</v>
       </c>
       <c r="I52">
-        <v>77.5</v>
+        <v>78.8</v>
       </c>
       <c r="J52">
-        <v>86</v>
+        <v>86.2</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2146,25 +2146,25 @@
         <v>35</v>
       </c>
       <c r="C54">
-        <v>63.1</v>
+        <v>63.6</v>
       </c>
       <c r="D54">
-        <v>75.2</v>
+        <v>74</v>
       </c>
       <c r="E54">
-        <v>68.90000000000001</v>
+        <v>67.5</v>
       </c>
       <c r="F54">
-        <v>73.2</v>
+        <v>72.7</v>
       </c>
       <c r="G54">
-        <v>67.3</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="H54">
-        <v>80.90000000000001</v>
+        <v>81.09999999999999</v>
       </c>
       <c r="I54">
-        <v>67.59999999999999</v>
+        <v>67.2</v>
       </c>
       <c r="J54">
         <v>74.8</v>
@@ -2208,25 +2208,25 @@
         <v>35</v>
       </c>
       <c r="C56">
-        <v>184.9</v>
+        <v>185.6</v>
       </c>
       <c r="D56">
-        <v>203.6</v>
+        <v>204</v>
       </c>
       <c r="E56">
-        <v>188.8</v>
+        <v>190.5</v>
       </c>
       <c r="F56">
-        <v>209.5</v>
+        <v>210.9</v>
       </c>
       <c r="G56">
-        <v>173.9</v>
+        <v>174.6</v>
       </c>
       <c r="H56">
-        <v>199.7</v>
+        <v>200.8</v>
       </c>
       <c r="I56">
-        <v>176.2</v>
+        <v>176.4</v>
       </c>
       <c r="J56">
         <v>182.1</v>
@@ -2273,25 +2273,25 @@
         <v>35.5</v>
       </c>
       <c r="D58">
-        <v>41.2</v>
+        <v>41.5</v>
       </c>
       <c r="E58">
-        <v>32.5</v>
+        <v>32.1</v>
       </c>
       <c r="F58">
-        <v>37.6</v>
+        <v>37.9</v>
       </c>
       <c r="G58">
-        <v>30.5</v>
+        <v>31.1</v>
       </c>
       <c r="H58">
-        <v>37.5</v>
+        <v>37.1</v>
       </c>
       <c r="I58">
-        <v>32.2</v>
+        <v>32.1</v>
       </c>
       <c r="J58">
-        <v>34.7</v>
+        <v>34.8</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2332,25 +2332,25 @@
         <v>35</v>
       </c>
       <c r="C60">
-        <v>157.1</v>
+        <v>157.5</v>
       </c>
       <c r="D60">
-        <v>194.5</v>
+        <v>191</v>
       </c>
       <c r="E60">
-        <v>172.7</v>
+        <v>172.4</v>
       </c>
       <c r="F60">
         <v>181.1</v>
       </c>
       <c r="G60">
-        <v>152.6</v>
+        <v>151.9</v>
       </c>
       <c r="H60">
-        <v>166.7</v>
+        <v>166.6</v>
       </c>
       <c r="I60">
-        <v>160.1</v>
+        <v>159.4</v>
       </c>
       <c r="J60">
         <v>163.3</v>
@@ -2394,25 +2394,25 @@
         <v>35</v>
       </c>
       <c r="C62">
-        <v>326.7</v>
+        <v>323.1</v>
       </c>
       <c r="D62">
-        <v>376</v>
+        <v>374.6</v>
       </c>
       <c r="E62">
-        <v>355.2</v>
+        <v>355.5</v>
       </c>
       <c r="F62">
-        <v>367.3</v>
+        <v>366.6</v>
       </c>
       <c r="G62">
-        <v>336.7</v>
+        <v>335.1</v>
       </c>
       <c r="H62">
-        <v>375.8</v>
+        <v>375.6</v>
       </c>
       <c r="I62">
-        <v>334.3</v>
+        <v>333.6</v>
       </c>
       <c r="J62">
         <v>374.7</v>
@@ -2456,22 +2456,22 @@
         <v>35</v>
       </c>
       <c r="C64">
-        <v>14.5</v>
+        <v>14.8</v>
       </c>
       <c r="D64">
-        <v>13.9</v>
+        <v>13.2</v>
       </c>
       <c r="E64">
-        <v>14</v>
+        <v>13.4</v>
       </c>
       <c r="F64">
-        <v>12.1</v>
+        <v>11.8</v>
       </c>
       <c r="G64">
         <v>19.4</v>
       </c>
       <c r="H64">
-        <v>19</v>
+        <v>18.7</v>
       </c>
       <c r="I64">
         <v>14.5</v>
@@ -2518,25 +2518,25 @@
         <v>35</v>
       </c>
       <c r="C66">
-        <v>18</v>
+        <v>17.3</v>
       </c>
       <c r="D66">
         <v>20.3</v>
       </c>
       <c r="E66">
-        <v>16.5</v>
+        <v>15.7</v>
       </c>
       <c r="F66">
         <v>22.3</v>
       </c>
       <c r="G66">
-        <v>24.9</v>
+        <v>25.7</v>
       </c>
       <c r="H66">
         <v>21.5</v>
       </c>
       <c r="I66">
-        <v>20.3</v>
+        <v>20.1</v>
       </c>
       <c r="J66">
         <v>19.3</v>

</xml_diff>